<commit_message>
fix minor: 1. Employee Edit view error on registered date 2. Employee landing search keywords 3. Upload Setting file not well text form when open in notepad 4. Upload template file. 4. Try fixing employee attendance finger error view with uploading new timepicker.js with valid semicolon
</commit_message>
<xml_diff>
--- a/system/storage/app/my/bauk/attendance/employee_attendance.xlsx
+++ b/system/storage/app/my/bauk/attendance/employee_attendance.xlsx
@@ -39,10 +39,10 @@
     <t>Finger Keluar 3</t>
   </si>
   <si>
-    <t>11-22-2019</t>
-  </si>
-  <si>
     <t>Kehadiran Finger</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -114,17 +114,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,117 +412,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
         <v>12345678</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="12">
+        <v>43810</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.47387731481481482</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="14">
+        <v>43801</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.4583564814814815</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.47387731481481482</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>